<commit_message>
Style: Apply professional formatting (bold headers, currency, auto-width) to Excel report
</commit_message>
<xml_diff>
--- a/January_Closing_Report.xlsx
+++ b/January_Closing_Report.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +57,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,6 +435,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -471,7 +480,7 @@
           <t>Software Subscription</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2" t="n">
         <v>52.99</v>
       </c>
     </row>
@@ -491,7 +500,7 @@
           <t>Office Supplies</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="2" t="n">
         <v>124.5</v>
       </c>
     </row>
@@ -511,7 +520,7 @@
           <t>Software Subscription</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -531,7 +540,7 @@
           <t>Meals &amp; Entertainment</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="2" t="n">
         <v>65.2</v>
       </c>
     </row>
@@ -551,7 +560,7 @@
           <t>Software Subscription</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="2" t="n">
         <v>34.15</v>
       </c>
     </row>

</xml_diff>